<commit_message>
v3.1.3-Stabilisation du module-Revue export des adhérents filtrés
Revue des différents scripts pour stabiliser vs(SPIP3.1)
Correction problématiques de séléctions des saisons actives en export.
</commit_message>
<xml_diff>
--- a/documentation/adhclub_enchainements.xlsx
+++ b/documentation/adhclub_enchainements.xlsx
@@ -5,167 +5,195 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="i3_adherents - Site Prive" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="adh_tous - Site Prive" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="adh_tous - Site Public" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="adhsaison - Site Prive" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="exec-adh_adherents - Site Prive" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="adh_tous - Site Prive" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="adh_tous - Site Public" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="adhsaison - Site Prive" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
-    <t>exec/inscription3_adherents.php/F(exec_inscription3_adherents)</t>
+    <t xml:space="preserve">exec/inscription3_adherents.php/F(exec_inscription3_adherents)</t>
   </si>
   <si>
-    <t>inc/commencer_page(inscription3:gestion_adherents)</t>
+    <t xml:space="preserve">inc/commencer_page(inscription3:gestion_adherents)</t>
   </si>
   <si>
-    <t>gros_titre(adhclub:titre_adhclub)</t>
+    <t xml:space="preserve">gros_titre(adhclub:titre_adhclub)</t>
   </si>
   <si>
-    <t>prive/table_adherents.html</t>
+    <t xml:space="preserve">prive/table_adherents.html</t>
   </si>
   <si>
-    <t>inscription3:descriptif_plugin</t>
+    <t xml:space="preserve">inscription3:descriptif_plugin</t>
   </si>
   <si>
-    <t>formulaire/inscription3_recherche.html</t>
+    <t xml:space="preserve">formulaire/inscription3_recherche.html</t>
   </si>
   <si>
-    <t>Saisie du Critère</t>
+    <t xml:space="preserve">Saisie du Critère</t>
   </si>
   <si>
-    <t>prive/formulaires/inscription3_recherche_cas</t>
+    <t xml:space="preserve">prive/formulaires/inscription3_recherche_cas</t>
   </si>
   <si>
-    <t>prive/menu_inscription3</t>
+    <t xml:space="preserve">prive/menu_inscription3</t>
   </si>
   <si>
-    <t>Choix du champ</t>
+    <t xml:space="preserve">Choix du champ</t>
   </si>
   <si>
-    <t>Bt Afficher  Tous</t>
+    <t xml:space="preserve">Bt Afficher  Tous</t>
   </si>
   <si>
-    <t>Bt Recherche</t>
+    <t xml:space="preserve">Bt Recherche</t>
   </si>
   <si>
-    <t>prive/table_adherent_auteur_recherche.html</t>
+    <t xml:space="preserve">prive/table_adherent_auteur_recherche.html</t>
   </si>
   <si>
-    <t>ou</t>
+    <t xml:space="preserve">ou</t>
   </si>
   <si>
-    <t>prive/adh_legend_droite</t>
+    <t xml:space="preserve">prive/adh_legend_droite</t>
   </si>
   <si>
-    <t>prive/table_adherent_auteur.html</t>
+    <t xml:space="preserve">prive/table_adherent_auteur.html</t>
   </si>
   <si>
-    <t>Bt Supprimer le(s) utilisateurs sélectionné(s)</t>
+    <t xml:space="preserve">Bt Supprimer le(s) utilisateurs sélectionné(s)</t>
   </si>
   <si>
-    <t>exec/adh_tous.php/F(exec_adh_tous)</t>
+    <t xml:space="preserve">prive/squelettes/top/adh_adherents.html</t>
   </si>
   <si>
-    <t>inc/commencer_page(adhclub:adhclub)</t>
+    <t xml:space="preserve">prive/squelettes/contenu/adh_adherents.html</t>
   </si>
   <si>
-    <t>prive/adh_adherents.html</t>
+    <t xml:space="preserve">h1(adhclub:liste_comptes_titre)</t>
   </si>
   <si>
-    <t>h1(adhclub:liste_comptes_titre)</t>
+    <t xml:space="preserve">prive/adh_menu_tous.html</t>
   </si>
   <si>
-    <t>prive/adh_menu_tous.html</t>
+    <t xml:space="preserve">Si type_objet &amp; id_objet</t>
   </si>
   <si>
-    <t>Si type_objet &amp; id_objet</t>
+    <t xml:space="preserve">h1(adhclub:mailer_envoi)</t>
   </si>
   <si>
-    <t>h1(adhclub:mailer_envoi)</t>
+    <t xml:space="preserve">exec/adh_saison</t>
   </si>
   <si>
-    <t>exec/adh_saison</t>
+    <t xml:space="preserve">Si type_objet article</t>
   </si>
   <si>
-    <t>Si type_objet article</t>
+    <t xml:space="preserve">exec/adh_assur</t>
   </si>
   <si>
-    <t>exec/adh_assur</t>
+    <t xml:space="preserve">public/inclure/adh_article</t>
   </si>
   <si>
-    <t>public/adh_article</t>
+    <t xml:space="preserve">exec/adh_coti</t>
   </si>
   <si>
-    <t>exec/adh_coti</t>
+    <t xml:space="preserve">exec/adh_niveau</t>
   </si>
   <si>
-    <t>exec/adh_niveau</t>
+    <t xml:space="preserve">exec/adh_import</t>
   </si>
   <si>
-    <t>exec/adh_import</t>
+    <t xml:space="preserve">formulaire/adh_i3_recherche.html</t>
   </si>
   <si>
-    <t>formulaire/adh_i3_recherche.html</t>
+    <t xml:space="preserve">Saisie des Critères Adh (Saison, etc..)</t>
   </si>
   <si>
-    <t>Saisie des Critères Adh</t>
+    <t xml:space="preserve">Choix du champ et saisie valeur</t>
   </si>
   <si>
-    <t>Choix du champ et saisie valeur</t>
+    <t xml:space="preserve">prive/inclure/adh_auteurs_recherche</t>
   </si>
   <si>
-    <t>prive/adh_auteur_recherche.html</t>
+    <t xml:space="preserve">prive/adh_auteur_recherche.html</t>
   </si>
   <si>
-    <t>Si espace privé</t>
+    <t xml:space="preserve">Si espace privé</t>
   </si>
   <si>
-    <t>Bt Exporter_liste.</t>
+    <t xml:space="preserve">Bt Exporter_liste.</t>
   </si>
   <si>
-    <t>Bt Mailer la Sélect.</t>
+    <t xml:space="preserve">Bt Mailer la Sélect.</t>
   </si>
   <si>
-    <t>modeles/adh_mailtous.html</t>
+    <t xml:space="preserve">exec/adh_tous.php/F(exec_adh_tous)</t>
   </si>
   <si>
-    <t>public/adh_tous.html</t>
+    <t xml:space="preserve">inc/commencer_page(adhclub:adhclub)</t>
   </si>
   <si>
-    <t>inc-head.html</t>
+    <t xml:space="preserve">prive/adh_adherents.html</t>
   </si>
   <si>
-    <t>inc-entete.html</t>
+    <t xml:space="preserve">public/adh_article</t>
   </si>
   <si>
-    <t>inc-rubrique.html</t>
+    <t xml:space="preserve">Saisie des Critères Adh</t>
   </si>
   <si>
-    <t>public/adh_adherents.html</t>
+    <t xml:space="preserve">modeles/adh_mailtous.html</t>
   </si>
   <si>
-    <t>prive/table_adherent_auteur_recherche</t>
+    <t xml:space="preserve">public/adh_tous.html</t>
   </si>
   <si>
-    <t>prive/table_adherent_auteur</t>
+    <t xml:space="preserve">inc-head.html</t>
   </si>
   <si>
-    <t>inc-pied.html</t>
+    <t xml:space="preserve">inc-entete.html</t>
   </si>
   <si>
-    <t>paquet.xml</t>
+    <t xml:space="preserve">inc-rubrique.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public/adh_adherents.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prive/table_adherent_auteur_recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prive/table_adherent_auteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inc-pied.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paquet.xml</t>
   </si>
   <si>
     <r>
-      <t>    </t>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF3C3C3C"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
     </r>
     <r>
       <rPr>
@@ -173,8 +201,9 @@
         <color rgb="FF008080"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>&lt;</t>
+      <t xml:space="preserve">&lt;</t>
     </r>
     <r>
       <rPr>
@@ -182,8 +211,9 @@
         <color rgb="FF3F7F7F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>menu</t>
+      <t xml:space="preserve">menu</t>
     </r>
     <r>
       <rPr>
@@ -192,7 +222,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -200,8 +230,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>nom</t>
+      <t xml:space="preserve">nom</t>
     </r>
     <r>
       <rPr>
@@ -209,8 +240,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -219,8 +251,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"adh_adherents"</t>
+      <t xml:space="preserve">"adh_adherents"</t>
     </r>
     <r>
       <rPr>
@@ -229,12 +262,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
     <r>
-      <t>    	</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">    	</t>
     </r>
     <r>
       <rPr>
@@ -242,8 +281,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>action</t>
+      <t xml:space="preserve">action</t>
     </r>
     <r>
       <rPr>
@@ -251,8 +291,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -261,13 +302,20 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"adh_adherents"</t>
+      <t xml:space="preserve">"adh_adherents"</t>
     </r>
   </si>
   <si>
     <r>
-      <t>    	</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">    	</t>
     </r>
     <r>
       <rPr>
@@ -275,8 +323,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>titre</t>
+      <t xml:space="preserve">titre</t>
     </r>
     <r>
       <rPr>
@@ -284,8 +333,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -294,8 +344,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"adhclub:adhclub_titre"</t>
+      <t xml:space="preserve">"adhclub:adhclub_titre"</t>
     </r>
     <r>
       <rPr>
@@ -304,12 +355,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
     <r>
-      <t>    	</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">    	</t>
     </r>
     <r>
       <rPr>
@@ -317,8 +374,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>parent</t>
+      <t xml:space="preserve">parent</t>
     </r>
     <r>
       <rPr>
@@ -326,8 +384,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -336,8 +395,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"menu_edition"</t>
+      <t xml:space="preserve">"menu_edition"</t>
     </r>
     <r>
       <rPr>
@@ -346,12 +406,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
     <r>
-      <t>    	</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">    	</t>
     </r>
     <r>
       <rPr>
@@ -359,8 +425,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>icone</t>
+      <t xml:space="preserve">icone</t>
     </r>
     <r>
       <rPr>
@@ -368,8 +435,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -378,8 +446,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"images/adhclub-24.png"</t>
+      <t xml:space="preserve">"images/adhclub-24.png"</t>
     </r>
     <r>
       <rPr>
@@ -388,7 +457,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -396,16 +465,24 @@
         <color rgb="FF008080"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>/&gt;</t>
+      <t xml:space="preserve">/&gt;</t>
     </r>
   </si>
   <si>
-    <t> </t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <r>
-      <t>	</t>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF3C3C3C"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">	</t>
     </r>
     <r>
       <rPr>
@@ -413,8 +490,9 @@
         <color rgb="FF008080"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>&lt;</t>
+      <t xml:space="preserve">&lt;</t>
     </r>
     <r>
       <rPr>
@@ -422,8 +500,9 @@
         <color rgb="FF3F7F7F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>onglet</t>
+      <t xml:space="preserve">onglet</t>
     </r>
     <r>
       <rPr>
@@ -432,7 +511,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -440,8 +519,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>nom</t>
+      <t xml:space="preserve">nom</t>
     </r>
     <r>
       <rPr>
@@ -449,8 +529,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -459,8 +540,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"adhsaisons"</t>
+      <t xml:space="preserve">"adhsaisons"</t>
     </r>
     <r>
       <rPr>
@@ -469,7 +551,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -477,8 +559,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>titre</t>
+      <t xml:space="preserve">titre</t>
     </r>
     <r>
       <rPr>
@@ -486,8 +569,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -496,8 +580,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"adhsaison:icone_menu_adhsaison"</t>
+      <t xml:space="preserve">"adhsaison:icone_menu_adhsaison"</t>
     </r>
     <r>
       <rPr>
@@ -506,7 +591,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -514,8 +599,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>parent</t>
+      <t xml:space="preserve">parent</t>
     </r>
     <r>
       <rPr>
@@ -523,8 +609,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -533,8 +620,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"adh_adherents"</t>
+      <t xml:space="preserve">"adh_adherents"</t>
     </r>
     <r>
       <rPr>
@@ -543,7 +631,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -551,8 +639,9 @@
         <color rgb="FF7F007F"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>action</t>
+      <t xml:space="preserve">action</t>
     </r>
     <r>
       <rPr>
@@ -560,8 +649,9 @@
         <color rgb="FF3C3C3C"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>=</t>
+      <t xml:space="preserve">=</t>
     </r>
     <r>
       <rPr>
@@ -570,8 +660,9 @@
         <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>"adhsaisons"</t>
+      <t xml:space="preserve">"adhsaisons"</t>
     </r>
     <r>
       <rPr>
@@ -580,7 +671,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -588,48 +679,49 @@
         <color rgb="FF008080"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t>/&gt;</t>
+      <t xml:space="preserve">/&gt;</t>
     </r>
   </si>
   <si>
-    <t>prive/squelette/top/adhsaisons.html</t>
+    <t xml:space="preserve">prive/squelette/top/adhsaisons.html</t>
   </si>
   <si>
-    <t>[(#VAL{adh_adherents}|barre_onglets{adhsaisons})]</t>
+    <t xml:space="preserve">[(#VAL{adh_adherents}|barre_onglets{adhsaisons})]</t>
   </si>
   <si>
-    <t>prive/squelette/navigation/adhsaisons.html</t>
+    <t xml:space="preserve">prive/squelette/navigation/adhsaisons.html</t>
   </si>
   <si>
-    <t>prive/squelette/contenu/adhsaisons.html</t>
+    <t xml:space="preserve">prive/squelette/contenu/adhsaisons.html</t>
   </si>
   <si>
-    <t>adhsaison:page_info_adhsaison</t>
+    <t xml:space="preserve">adhsaison:page_info_adhsaison</t>
   </si>
   <si>
-    <t>h1(adhsaison:titre_adhsaisons)</t>
+    <t xml:space="preserve">h1(adhsaison:titre_adhsaisons)</t>
   </si>
   <si>
-    <t>prive/objets/liste/adhsaisons.html</t>
+    <t xml:space="preserve">prive/objets/liste/adhsaisons.html</t>
   </si>
   <si>
-    <t>#AUTORISER{modifier,adhsaison,#ID_SAISON}</t>
+    <t xml:space="preserve">#AUTORISER{modifier,adhsaison,#ID_SAISON}</t>
   </si>
   <si>
-    <t>formulaire/editer_adhsaison.html(#ID_SAISON)</t>
+    <t xml:space="preserve">formulaire/editer_adhsaison.html(#ID_SAISON)</t>
   </si>
   <si>
-    <t>#AUTORISER{supprimer,adhsaison,#ID_SAISON}</t>
+    <t xml:space="preserve">#AUTORISER{supprimer,adhsaison,#ID_SAISON}</t>
   </si>
   <si>
-    <t>action/supprimer_adhsaison.php(#ID_SAISON)</t>
+    <t xml:space="preserve">action/supprimer_adhsaison.php(#ID_SAISON)</t>
   </si>
   <si>
-    <t>#AUTORISER{modifier,adhsaison}</t>
+    <t xml:space="preserve">#AUTORISER{modifier,adhsaison}</t>
   </si>
   <si>
-    <t>formulaire/editer_adhsaison.html(new)</t>
+    <t xml:space="preserve">formulaire/editer_adhsaison.html(new)</t>
   </si>
 </sst>
 </file>
@@ -637,9 +729,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -699,28 +791,39 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF3C3C3C"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF008080"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF3F7F7F"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF7F007F"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -728,6 +831,7 @@
       <color rgb="FF2A00FF"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -940,7 +1044,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="94">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1109,6 +1213,46 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1121,24 +1265,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1173,14 +1337,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1205,11 +1361,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1217,11 +1369,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1249,18 +1401,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1273,7 +1417,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1371,7 +1515,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5316840" y="3136320"/>
+          <a:off x="5060160" y="3136320"/>
           <a:ext cx="0" cy="181440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1385,6 +1529,12 @@
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1408,8 +1558,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5478840" y="4241520"/>
-          <a:ext cx="465840" cy="0"/>
+          <a:off x="5222160" y="4241520"/>
+          <a:ext cx="411120" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1422,6 +1572,12 @@
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1445,7 +1601,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5459760" y="3984480"/>
+          <a:off x="5203080" y="3984480"/>
           <a:ext cx="0" cy="257040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1458,6 +1614,12 @@
           <a:round/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1465,6 +1627,309 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>760680</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>59040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>760680</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13079520" y="3641040"/>
+          <a:ext cx="0" cy="181080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>472320</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>41040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>150480</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>41040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13574880" y="4765320"/>
+          <a:ext cx="461520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>150480</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>100440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>150480</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>31320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14036400" y="4498200"/>
+          <a:ext cx="0" cy="257400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>687960</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1149480</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4418280" y="6169680"/>
+          <a:ext cx="461520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>677520</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>677520</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4407840" y="4915080"/>
+          <a:ext cx="0" cy="1231560"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>309960</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>771480</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7350120" y="5728680"/>
+          <a:ext cx="461520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>750240</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>82440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>763200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7790400" y="4961520"/>
+          <a:ext cx="12960" cy="767160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
@@ -1481,12 +1946,12 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Line 1"/>
+        <xdr:cNvPr id="10" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13729320" y="3641040"/>
+          <a:off x="13079520" y="3641040"/>
           <a:ext cx="0" cy="181080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1500,6 +1965,12 @@
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1518,13 +1989,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Line 1"/>
+        <xdr:cNvPr id="11" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14224680" y="4765320"/>
-          <a:ext cx="494280" cy="0"/>
+          <a:off x="13574880" y="4765320"/>
+          <a:ext cx="461520" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1537,6 +2008,12 @@
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1555,12 +2032,12 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Line 1"/>
+        <xdr:cNvPr id="12" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="14224680" y="4498200"/>
+          <a:off x="13574880" y="4498200"/>
           <a:ext cx="0" cy="257400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1573,6 +2050,12 @@
           <a:round/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1591,12 +2074,12 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Line 1"/>
+        <xdr:cNvPr id="13" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5030280" y="2993760"/>
+          <a:off x="4808520" y="2993760"/>
           <a:ext cx="0" cy="180720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1610,35 +2093,41 @@
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>779400</xdr:colOff>
+      <xdr:colOff>170280</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>779400</xdr:colOff>
+      <xdr:colOff>170280</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Line 1"/>
+        <xdr:cNvPr id="14" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5488560" y="3736440"/>
+          <a:off x="5230440" y="3736440"/>
           <a:ext cx="0" cy="171360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1652,31 +2141,37 @@
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>582480</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Line 1"/>
+        <xdr:cNvPr id="15" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5478840" y="4622400"/>
-          <a:ext cx="476280" cy="0"/>
+          <a:off x="5220720" y="4622400"/>
+          <a:ext cx="421920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1689,30 +2184,36 @@
           <a:tailEnd len="med" type="triangle" w="med"/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>152640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Line 1"/>
+        <xdr:cNvPr id="16" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5478840" y="4355640"/>
+          <a:off x="5220720" y="4355640"/>
           <a:ext cx="0" cy="266760"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1725,6 +2226,12 @@
           <a:round/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1739,22 +2246,21 @@
   <dimension ref="B1:Q39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.1479591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="14" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.1938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.5816326530612"/>
+    <col collapsed="false" hidden="false" max="17" min="14" style="0" width="2.31122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2502,26 +3008,1324 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
+  <dimension ref="B1:W55"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V40" activeCellId="0" sqref="V40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="10.9540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="35" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="17" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="1008" min="21" style="35" width="11.1071428571429"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4"/>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="0"/>
+      <c r="V6" s="0"/>
+      <c r="W6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="39"/>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="41"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="0"/>
+      <c r="W12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="21"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="21"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="22"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="22"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="22"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="45"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="0"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="40"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="40"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" s="27"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="59"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="61"/>
+      <c r="P33" s="61"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="40"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="40"/>
+      <c r="S35" s="40"/>
+      <c r="T35" s="40"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="40"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="O37" s="32"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
+      <c r="T37" s="40"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="40"/>
+      <c r="S38" s="40"/>
+      <c r="T38" s="40"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="40"/>
+      <c r="S39" s="40"/>
+      <c r="T39" s="40"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="63"/>
+      <c r="R40" s="40"/>
+      <c r="S40" s="40"/>
+      <c r="T40" s="40"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="64"/>
+      <c r="M41" s="64"/>
+      <c r="N41" s="64"/>
+      <c r="O41" s="64"/>
+      <c r="P41" s="64"/>
+      <c r="Q41" s="64"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+      <c r="T41" s="40"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="64"/>
+      <c r="N42" s="64"/>
+      <c r="O42" s="64"/>
+      <c r="P42" s="64"/>
+      <c r="Q42" s="64"/>
+      <c r="R42" s="40"/>
+      <c r="S42" s="40"/>
+      <c r="T42" s="40"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="40"/>
+      <c r="S43" s="40"/>
+      <c r="T43" s="40"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="65"/>
+      <c r="N44" s="37"/>
+      <c r="O44" s="37"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="40"/>
+      <c r="S44" s="40"/>
+      <c r="T44" s="40"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="40"/>
+      <c r="R45" s="40"/>
+      <c r="S45" s="40"/>
+      <c r="T45" s="40"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="66"/>
+      <c r="R46" s="40"/>
+      <c r="S46" s="40"/>
+      <c r="T46" s="40"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="67"/>
+      <c r="P47" s="68"/>
+      <c r="Q47" s="69"/>
+      <c r="R47" s="40"/>
+      <c r="S47" s="40"/>
+      <c r="T47" s="40"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="41"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="26"/>
+      <c r="R48" s="40"/>
+      <c r="S48" s="40"/>
+      <c r="T48" s="40"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="65"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="40"/>
+      <c r="S49" s="40"/>
+      <c r="T49" s="40"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="41"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="O50" s="21"/>
+      <c r="P50" s="21"/>
+      <c r="Q50" s="40"/>
+      <c r="R50" s="40"/>
+      <c r="S50" s="40"/>
+      <c r="T50" s="40"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="O51" s="27"/>
+      <c r="P51" s="27"/>
+      <c r="Q51" s="66"/>
+      <c r="R51" s="40"/>
+      <c r="S51" s="40"/>
+      <c r="T51" s="40"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="67"/>
+      <c r="O52" s="67"/>
+      <c r="P52" s="68"/>
+      <c r="Q52" s="69"/>
+      <c r="R52" s="40"/>
+      <c r="S52" s="40"/>
+      <c r="T52" s="40"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="53"/>
+      <c r="M53" s="53"/>
+      <c r="N53" s="53"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="53"/>
+      <c r="Q53" s="53"/>
+      <c r="R53" s="54"/>
+      <c r="S53" s="40"/>
+      <c r="T53" s="40"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="41"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="53"/>
+      <c r="L54" s="53"/>
+      <c r="M54" s="53"/>
+      <c r="N54" s="53"/>
+      <c r="O54" s="53"/>
+      <c r="P54" s="53"/>
+      <c r="Q54" s="53"/>
+      <c r="R54" s="53"/>
+      <c r="S54" s="54"/>
+      <c r="T54" s="40"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="52"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+      <c r="L55" s="53"/>
+      <c r="M55" s="53"/>
+      <c r="N55" s="53"/>
+      <c r="O55" s="53"/>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="53"/>
+      <c r="R55" s="53"/>
+      <c r="S55" s="53"/>
+      <c r="T55" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="J12:Q12"/>
+    <mergeCell ref="L18:Q18"/>
+    <mergeCell ref="L26:Q26"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L33:P33"/>
+    <mergeCell ref="L35:P36"/>
+    <mergeCell ref="L38:P39"/>
+    <mergeCell ref="N46:P46"/>
+    <mergeCell ref="N51:P51"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;14&amp;F - &amp;A</oddHeader>
+    <oddFooter>&amp;Ljremond&amp;CPage &amp;P&amp;R&amp;D</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
   <dimension ref="B1:V48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U14" activeCellId="0" sqref="U14"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="11.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="35" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="35" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="35" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="16" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="1007" min="20" style="35" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="1008" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="10.9540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="16" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="1007" min="20" style="35" width="11.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2573,7 +4377,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="39"/>
       <c r="C3" s="5" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2645,7 +4449,7 @@
       <c r="B6" s="41"/>
       <c r="C6" s="39"/>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2668,22 +4472,22 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="44"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="54"/>
       <c r="S7" s="40"/>
       <c r="T7" s="0"/>
       <c r="U7" s="0"/>
@@ -2739,7 +4543,7 @@
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="5" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -2770,7 +4574,7 @@
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
       <c r="J11" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -2779,8 +4583,8 @@
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
       <c r="T11" s="11"/>
       <c r="U11" s="0"/>
       <c r="V11" s="0"/>
@@ -2811,15 +4615,15 @@
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
-      <c r="E13" s="46" t="s">
-        <v>21</v>
+      <c r="E13" s="43" t="s">
+        <v>20</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="40"/>
       <c r="I13" s="26"/>
       <c r="J13" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K13" s="26"/>
       <c r="L13" s="26"/>
@@ -2842,7 +4646,7 @@
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
       <c r="K14" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
@@ -2879,13 +4683,13 @@
       <c r="D16" s="41"/>
       <c r="E16" s="20"/>
       <c r="F16" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="40"/>
       <c r="I16" s="26"/>
       <c r="J16" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
@@ -2903,21 +4707,21 @@
       <c r="D17" s="41"/>
       <c r="E17" s="20"/>
       <c r="F17" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="40"/>
       <c r="I17" s="26"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="49"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="47"/>
       <c r="R17" s="40"/>
       <c r="S17" s="40"/>
     </row>
@@ -2927,7 +4731,7 @@
       <c r="D18" s="41"/>
       <c r="E18" s="20"/>
       <c r="F18" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="40"/>
@@ -2949,7 +4753,7 @@
       <c r="D19" s="41"/>
       <c r="E19" s="20"/>
       <c r="F19" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="40"/>
@@ -2971,14 +4775,14 @@
       <c r="D20" s="41"/>
       <c r="E20" s="20"/>
       <c r="F20" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="40"/>
       <c r="I20" s="26"/>
       <c r="J20" s="39"/>
       <c r="K20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -3022,7 +4826,7 @@
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
       <c r="M22" s="14" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="N22" s="26"/>
       <c r="O22" s="26"/>
@@ -3034,11 +4838,11 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
       <c r="I23" s="26"/>
       <c r="J23" s="41"/>
       <c r="K23" s="26"/>
@@ -3108,7 +4912,7 @@
       <c r="K26" s="20"/>
       <c r="L26" s="21"/>
       <c r="M26" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
@@ -3120,11 +4924,11 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="44"/>
+      <c r="H27" s="54"/>
       <c r="I27" s="26"/>
       <c r="J27" s="41"/>
       <c r="K27" s="23"/>
@@ -3338,7 +5142,7 @@
       <c r="I37" s="26"/>
       <c r="J37" s="41"/>
       <c r="K37" s="26"/>
-      <c r="L37" s="50"/>
+      <c r="L37" s="65"/>
       <c r="M37" s="37"/>
       <c r="N37" s="37"/>
       <c r="O37" s="37"/>
@@ -3386,7 +5190,7 @@
       </c>
       <c r="N39" s="27"/>
       <c r="O39" s="27"/>
-      <c r="P39" s="51"/>
+      <c r="P39" s="66"/>
       <c r="Q39" s="40"/>
       <c r="R39" s="40"/>
       <c r="S39" s="40"/>
@@ -3402,11 +5206,11 @@
       <c r="I40" s="26"/>
       <c r="J40" s="41"/>
       <c r="K40" s="26"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="53"/>
-      <c r="P40" s="54"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="67"/>
+      <c r="N40" s="67"/>
+      <c r="O40" s="68"/>
+      <c r="P40" s="69"/>
       <c r="Q40" s="40"/>
       <c r="R40" s="40"/>
       <c r="S40" s="40"/>
@@ -3442,7 +5246,7 @@
       <c r="I42" s="26"/>
       <c r="J42" s="41"/>
       <c r="K42" s="26"/>
-      <c r="L42" s="50"/>
+      <c r="L42" s="65"/>
       <c r="M42" s="37"/>
       <c r="N42" s="37"/>
       <c r="O42" s="37"/>
@@ -3464,7 +5268,7 @@
       <c r="K43" s="26"/>
       <c r="L43" s="41"/>
       <c r="M43" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N43" s="21"/>
       <c r="O43" s="21"/>
@@ -3490,7 +5294,7 @@
       </c>
       <c r="N44" s="27"/>
       <c r="O44" s="27"/>
-      <c r="P44" s="51"/>
+      <c r="P44" s="66"/>
       <c r="Q44" s="40"/>
       <c r="R44" s="40"/>
       <c r="S44" s="40"/>
@@ -3506,11 +5310,11 @@
       <c r="I45" s="26"/>
       <c r="J45" s="41"/>
       <c r="K45" s="26"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="53"/>
-      <c r="P45" s="54"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="68"/>
+      <c r="P45" s="69"/>
       <c r="Q45" s="40"/>
       <c r="R45" s="40"/>
       <c r="S45" s="40"/>
@@ -3524,56 +5328,56 @@
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="43"/>
-      <c r="P46" s="43"/>
-      <c r="Q46" s="44"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="53"/>
+      <c r="M46" s="53"/>
+      <c r="N46" s="53"/>
+      <c r="O46" s="53"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="54"/>
       <c r="R46" s="40"/>
       <c r="S46" s="40"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="41"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="43"/>
-      <c r="P47" s="43"/>
-      <c r="Q47" s="43"/>
-      <c r="R47" s="44"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
+      <c r="L47" s="53"/>
+      <c r="M47" s="53"/>
+      <c r="N47" s="53"/>
+      <c r="O47" s="53"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="54"/>
       <c r="S47" s="40"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="42"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
-      <c r="M48" s="43"/>
-      <c r="N48" s="43"/>
-      <c r="O48" s="43"/>
-      <c r="P48" s="43"/>
-      <c r="Q48" s="43"/>
-      <c r="R48" s="43"/>
-      <c r="S48" s="44"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3592,7 +5396,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;14&amp;F - &amp;A</oddHeader>
     <oddFooter>&amp;Ljremond&amp;CPage &amp;P&amp;R&amp;D</oddFooter>
@@ -3601,7 +5405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
@@ -3609,22 +5413,21 @@
   <dimension ref="B2:S48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X19" activeCellId="0" sqref="X19"/>
+      <selection pane="topLeft" activeCell="W24" activeCellId="0" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.1479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="15" style="0" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.1224489795918"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.1224489795918"/>
+    <col collapsed="false" hidden="false" max="19" min="15" style="0" width="2.31122448979592"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3650,7 +5453,7 @@
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -3713,7 +5516,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3776,7 +5579,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -3797,18 +5600,18 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -3858,7 +5661,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -3879,18 +5682,18 @@
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="70"/>
+      <c r="P14" s="70"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
@@ -3952,7 +5755,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="3"/>
-      <c r="R17" s="56"/>
+      <c r="R17" s="71"/>
       <c r="S17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3960,13 +5763,13 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="6"/>
       <c r="H18" s="4"/>
       <c r="I18" s="12" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
@@ -3976,7 +5779,7 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="56"/>
+      <c r="R18" s="71"/>
       <c r="S18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3996,7 +5799,7 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="7"/>
-      <c r="R19" s="56"/>
+      <c r="R19" s="71"/>
       <c r="S19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4008,17 +5811,17 @@
       <c r="G20" s="6"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
+      <c r="J20" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="72"/>
+      <c r="L20" s="72"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="7"/>
-      <c r="R20" s="56"/>
+      <c r="R20" s="71"/>
       <c r="S20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4038,7 +5841,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
-      <c r="R21" s="56"/>
+      <c r="R21" s="71"/>
       <c r="S21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4060,7 +5863,7 @@
       <c r="O22" s="6"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
-      <c r="R22" s="56"/>
+      <c r="R22" s="71"/>
       <c r="S22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4080,7 +5883,7 @@
       <c r="O23" s="6"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
-      <c r="R23" s="56"/>
+      <c r="R23" s="71"/>
       <c r="S23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,7 +5903,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
-      <c r="R24" s="56"/>
+      <c r="R24" s="71"/>
       <c r="S24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4122,7 +5925,7 @@
       <c r="O25" s="18"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
-      <c r="R25" s="56"/>
+      <c r="R25" s="71"/>
       <c r="S25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4144,7 +5947,7 @@
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
-      <c r="R26" s="56"/>
+      <c r="R26" s="71"/>
       <c r="S26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4164,7 +5967,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
-      <c r="R27" s="56"/>
+      <c r="R27" s="71"/>
       <c r="S27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,7 +5987,7 @@
       <c r="O28" s="6"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
-      <c r="R28" s="56"/>
+      <c r="R28" s="71"/>
       <c r="S28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4208,7 +6011,7 @@
       <c r="O29" s="58"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
-      <c r="R29" s="56"/>
+      <c r="R29" s="71"/>
       <c r="S29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,7 +6023,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="59"/>
+      <c r="J30" s="57"/>
       <c r="K30" s="58"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -4228,7 +6031,7 @@
       <c r="O30" s="58"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
-      <c r="R30" s="56"/>
+      <c r="R30" s="71"/>
       <c r="S30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4241,7 +6044,7 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="31" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="K31" s="31"/>
       <c r="L31" s="31"/>
@@ -4250,7 +6053,7 @@
       <c r="O31" s="31"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
-      <c r="R31" s="56"/>
+      <c r="R31" s="71"/>
       <c r="S31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4270,7 +6073,7 @@
       <c r="O32" s="31"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
-      <c r="R32" s="56"/>
+      <c r="R32" s="71"/>
       <c r="S32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4292,7 +6095,7 @@
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
-      <c r="R33" s="56"/>
+      <c r="R33" s="71"/>
       <c r="S33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4305,7 +6108,7 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="33" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K34" s="33"/>
       <c r="L34" s="33"/>
@@ -4314,7 +6117,7 @@
       <c r="O34" s="33"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
-      <c r="R34" s="56"/>
+      <c r="R34" s="71"/>
       <c r="S34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,7 +6137,7 @@
       <c r="O35" s="33"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
-      <c r="R35" s="56"/>
+      <c r="R35" s="71"/>
       <c r="S35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4346,15 +6149,15 @@
       <c r="G36" s="6"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="60"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
-      <c r="R36" s="56"/>
+      <c r="R36" s="71"/>
       <c r="S36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4366,15 +6169,15 @@
       <c r="G37" s="6"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="61"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="74"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="3"/>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
-      <c r="R37" s="56"/>
+      <c r="R37" s="71"/>
       <c r="S37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4389,14 +6192,14 @@
       <c r="J38" s="6"/>
       <c r="K38" s="4"/>
       <c r="L38" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
-      <c r="R38" s="56"/>
+      <c r="R38" s="71"/>
       <c r="S38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4415,10 +6218,10 @@
       </c>
       <c r="M39" s="27"/>
       <c r="N39" s="27"/>
-      <c r="O39" s="62"/>
+      <c r="O39" s="75"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
-      <c r="R39" s="56"/>
+      <c r="R39" s="71"/>
       <c r="S39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4432,13 +6235,13 @@
       <c r="I40" s="4"/>
       <c r="J40" s="6"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="63"/>
-      <c r="M40" s="63"/>
-      <c r="N40" s="64"/>
-      <c r="O40" s="65"/>
+      <c r="L40" s="76"/>
+      <c r="M40" s="76"/>
+      <c r="N40" s="77"/>
+      <c r="O40" s="78"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
-      <c r="R40" s="56"/>
+      <c r="R40" s="71"/>
       <c r="S40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4458,7 +6261,7 @@
       <c r="O41" s="9"/>
       <c r="P41" s="10"/>
       <c r="Q41" s="7"/>
-      <c r="R41" s="56"/>
+      <c r="R41" s="71"/>
       <c r="S41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4478,7 +6281,7 @@
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="10"/>
-      <c r="R42" s="56"/>
+      <c r="R42" s="71"/>
       <c r="S42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,7 +6329,7 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -4547,18 +6350,18 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-      <c r="L46" s="55"/>
-      <c r="M46" s="55"/>
-      <c r="N46" s="55"/>
-      <c r="O46" s="55"/>
-      <c r="P46" s="55"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="70"/>
+      <c r="J46" s="70"/>
+      <c r="K46" s="70"/>
+      <c r="L46" s="70"/>
+      <c r="M46" s="70"/>
+      <c r="N46" s="70"/>
+      <c r="O46" s="70"/>
+      <c r="P46" s="70"/>
       <c r="Q46" s="10"/>
       <c r="R46" s="7"/>
       <c r="S46" s="7"/>
@@ -4566,7 +6369,7 @@
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="66"/>
+      <c r="D47" s="51"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -4630,31 +6433,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B1:Y44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="11.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="26.8112244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="35" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="35" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="35" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="22" min="19" style="35" width="2.57142857142857"/>
-    <col collapsed="false" hidden="false" max="1010" min="23" style="35" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="1011" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="10.9540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="35" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="22" min="19" style="35" width="2.31122448979592"/>
+    <col collapsed="false" hidden="false" max="1010" min="23" style="35" width="11.1071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4686,7 +6488,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0"/>
       <c r="C2" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
@@ -4713,8 +6515,8 @@
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0"/>
-      <c r="C3" s="67" t="s">
-        <v>48</v>
+      <c r="C3" s="79" t="s">
+        <v>53</v>
       </c>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
@@ -4741,8 +6543,8 @@
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0"/>
-      <c r="C4" s="68" t="s">
-        <v>49</v>
+      <c r="C4" s="80" t="s">
+        <v>54</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
@@ -4769,8 +6571,8 @@
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0"/>
-      <c r="C5" s="68" t="s">
-        <v>50</v>
+      <c r="C5" s="80" t="s">
+        <v>55</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
@@ -4797,8 +6599,8 @@
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0"/>
-      <c r="C6" s="68" t="s">
-        <v>51</v>
+      <c r="C6" s="80" t="s">
+        <v>56</v>
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
@@ -4825,8 +6627,8 @@
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0"/>
-      <c r="C7" s="68" t="s">
-        <v>52</v>
+      <c r="C7" s="80" t="s">
+        <v>57</v>
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
@@ -4853,8 +6655,8 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0"/>
-      <c r="C8" s="69" t="s">
-        <v>53</v>
+      <c r="C8" s="81" t="s">
+        <v>58</v>
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
@@ -4881,8 +6683,8 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0"/>
-      <c r="C9" s="67" t="s">
-        <v>54</v>
+      <c r="C9" s="79" t="s">
+        <v>59</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
@@ -4988,8 +6790,8 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
-      <c r="D13" s="46" t="s">
-        <v>55</v>
+      <c r="D13" s="43" t="s">
+        <v>60</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
@@ -5016,7 +6818,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
-      <c r="D14" s="46"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
@@ -5042,8 +6844,8 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
-      <c r="D15" s="69" t="s">
-        <v>56</v>
+      <c r="D15" s="81" t="s">
+        <v>61</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
@@ -5069,25 +6871,25 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="44"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="53"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="54"/>
       <c r="V16" s="40"/>
       <c r="W16" s="0"/>
       <c r="X16" s="0"/>
@@ -5096,7 +6898,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="41"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="69"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
@@ -5121,13 +6923,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="39"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="73"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="85"/>
       <c r="J18" s="5"/>
       <c r="K18" s="1"/>
       <c r="L18" s="2"/>
@@ -5147,43 +6949,43 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="41"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="75" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="76"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="88"/>
       <c r="J19" s="26"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="77" t="s">
-        <v>58</v>
-      </c>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77"/>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="77"/>
-      <c r="S19" s="77"/>
-      <c r="T19" s="77"/>
+      <c r="L19" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="87"/>
+      <c r="R19" s="87"/>
+      <c r="S19" s="87"/>
+      <c r="T19" s="87"/>
       <c r="U19" s="7"/>
-      <c r="V19" s="45"/>
+      <c r="V19" s="42"/>
       <c r="W19" s="11"/>
       <c r="X19" s="0"/>
       <c r="Y19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="41"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="46"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="43"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
-      <c r="I20" s="76"/>
+      <c r="I20" s="88"/>
       <c r="J20" s="26"/>
       <c r="K20" s="4"/>
       <c r="L20" s="0"/>
@@ -5203,28 +7005,28 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="41"/>
-      <c r="C21" s="78"/>
+      <c r="C21" s="89"/>
       <c r="D21" s="11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="76"/>
+      <c r="I21" s="88"/>
       <c r="J21" s="26"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="79"/>
-      <c r="S21" s="79"/>
-      <c r="T21" s="79"/>
+      <c r="L21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
       <c r="U21" s="7"/>
       <c r="V21" s="40"/>
       <c r="W21" s="0"/>
@@ -5233,13 +7035,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="41"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="82"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="92"/>
       <c r="J22" s="26"/>
       <c r="K22" s="4"/>
       <c r="L22" s="0"/>
@@ -5295,15 +7097,15 @@
       <c r="J24" s="0"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="75"/>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="75"/>
-      <c r="S24" s="75"/>
+      <c r="M24" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="N24" s="87"/>
+      <c r="O24" s="87"/>
+      <c r="P24" s="87"/>
+      <c r="Q24" s="87"/>
+      <c r="R24" s="87"/>
+      <c r="S24" s="87"/>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
       <c r="V24" s="40"/>
@@ -5349,15 +7151,15 @@
       <c r="J26" s="0"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="79" t="s">
-        <v>62</v>
-      </c>
-      <c r="N26" s="79"/>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="79"/>
+      <c r="M26" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
       <c r="V26" s="40"/>
@@ -5400,13 +7202,13 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="O28" s="79"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="79"/>
+      <c r="N28" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
       <c r="S28" s="7"/>
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
@@ -5470,15 +7272,15 @@
       <c r="J31" s="0"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="N31" s="79"/>
-      <c r="O31" s="79"/>
-      <c r="P31" s="79"/>
-      <c r="Q31" s="79"/>
-      <c r="R31" s="79"/>
-      <c r="S31" s="79"/>
+      <c r="M31" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
       <c r="V31" s="40"/>
@@ -5519,13 +7321,13 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="O33" s="79"/>
-      <c r="P33" s="79"/>
-      <c r="Q33" s="79"/>
-      <c r="R33" s="79"/>
+      <c r="N33" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
@@ -5590,12 +7392,12 @@
       <c r="K36" s="4"/>
       <c r="L36" s="0"/>
       <c r="M36" s="0"/>
-      <c r="N36" s="0"/>
-      <c r="O36" s="0"/>
-      <c r="P36" s="0"/>
-      <c r="Q36" s="0"/>
-      <c r="R36" s="0"/>
-      <c r="S36" s="0"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
       <c r="T36" s="0"/>
       <c r="U36" s="7"/>
       <c r="V36" s="40"/>
@@ -5611,17 +7413,17 @@
       <c r="I37" s="0"/>
       <c r="J37" s="0"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="83" t="s">
-        <v>66</v>
-      </c>
-      <c r="M37" s="83"/>
-      <c r="N37" s="83"/>
-      <c r="O37" s="83"/>
-      <c r="P37" s="83"/>
-      <c r="Q37" s="83"/>
-      <c r="R37" s="83"/>
-      <c r="S37" s="83"/>
-      <c r="T37" s="83"/>
+      <c r="L37" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="M37" s="93"/>
+      <c r="N37" s="93"/>
+      <c r="O37" s="93"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="93"/>
+      <c r="S37" s="93"/>
+      <c r="T37" s="93"/>
       <c r="U37" s="7"/>
       <c r="V37" s="40"/>
     </row>
@@ -5660,15 +7462,15 @@
       <c r="J39" s="0"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="N39" s="79"/>
-      <c r="O39" s="79"/>
-      <c r="P39" s="79"/>
-      <c r="Q39" s="79"/>
-      <c r="R39" s="79"/>
-      <c r="S39" s="79"/>
+      <c r="M39" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
       <c r="T39" s="7"/>
       <c r="U39" s="7"/>
       <c r="V39" s="40"/>
@@ -5732,8 +7534,8 @@
       <c r="K42" s="4"/>
       <c r="L42" s="0"/>
       <c r="M42" s="0"/>
-      <c r="N42" s="0"/>
-      <c r="O42" s="0"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
       <c r="P42" s="0"/>
       <c r="Q42" s="0"/>
       <c r="R42" s="0"/>
@@ -5766,27 +7568,27 @@
       <c r="V43" s="40"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="42"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43"/>
-      <c r="N44" s="43"/>
-      <c r="O44" s="43"/>
-      <c r="P44" s="43"/>
-      <c r="Q44" s="43"/>
-      <c r="R44" s="43"/>
-      <c r="S44" s="43"/>
-      <c r="T44" s="43"/>
-      <c r="U44" s="43"/>
-      <c r="V44" s="44"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="53"/>
+      <c r="R44" s="53"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>